<commit_message>
VERSION 2.0: NEW FIRMWARE UPDATED
- Now use from the custom STM32-driver
- Recode every projects, focusing on BOOTLOADER, APP_OLD, & APP_CURRENT
- Imported ESP32_to_STM32 folders
</commit_message>
<xml_diff>
--- a/STM32 DRIVERS ERRORS.xlsx
+++ b/STM32 DRIVERS ERRORS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\File_dai_hoc_UIT\Thuc_Tap_FSOFT\INTERN_PROJECT\STM32_BOOTLOADER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEA27E94-9679-4AAA-A26F-06F8D3DFD815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A27EAE4-8852-4EE0-9C45-0BD6A80A1A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{25A5A94A-9CA5-4519-BCB4-490A2B18D65F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="85">
   <si>
     <t>File</t>
   </si>
@@ -230,27 +230,6 @@
     <t>use of undeclared identifier 'SCB_AIRCR_SYSRESETREQ_Msk'</t>
   </si>
   <si>
-    <t>core_cm3.h</t>
-  </si>
-  <si>
-    <t>unknown type name 'IRQn_Type'</t>
-  </si>
-  <si>
-    <t>Missing device-specific header</t>
-  </si>
-  <si>
-    <t>Include device header (e.g., stm32f103xx.h)</t>
-  </si>
-  <si>
-    <t>use of undeclared identifier '__NVIC_PRIO_BITS'</t>
-  </si>
-  <si>
-    <t>Missing device-specific definition</t>
-  </si>
-  <si>
-    <t>Define __NVIC_PRIO_BITS or include device header</t>
-  </si>
-  <si>
     <t>stm32f103xx_gpio_drivers.c</t>
   </si>
   <si>
@@ -285,6 +264,33 @@
   </si>
   <si>
     <t>STM32 DRIVERS ERRORS</t>
+  </si>
+  <si>
+    <t>call to undeclared function 'USART_Enable'</t>
+  </si>
+  <si>
+    <t>Missing function declaration in driver</t>
+  </si>
+  <si>
+    <t>bootloader.c</t>
+  </si>
+  <si>
+    <t>call to undeclared function '__disable_irq'</t>
+  </si>
+  <si>
+    <t>Missing CMSIS function, avoided by design</t>
+  </si>
+  <si>
+    <t>call to undeclared function '__set_MSP'</t>
+  </si>
+  <si>
+    <t>Missing CMSIS function, replaced with asm</t>
+  </si>
+  <si>
+    <t>call to undeclared function '__enable_irq'</t>
+  </si>
+  <si>
+    <t>Stubbed struct visibility</t>
   </si>
 </sst>
 </file>
@@ -681,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AA74CDA-4D94-451C-BB38-A47B807C0E06}">
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="41.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -699,7 +705,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1492,419 +1498,204 @@
         <v>64</v>
       </c>
       <c r="B41" s="2">
-        <v>1612</v>
+        <v>69</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B42" s="2">
-        <v>1631</v>
+        <v>22</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B43" s="2">
-        <v>1650</v>
+        <v>155</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B44" s="2">
-        <v>1669</v>
+        <v>171</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B45" s="2">
-        <v>1688</v>
+        <v>201</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B46" s="2">
-        <v>1703</v>
+        <v>270</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B47" s="2">
-        <v>1720</v>
+        <v>331</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B48" s="2">
-        <v>1742</v>
+        <v>29</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B49" s="2">
-        <v>1746</v>
+        <v>30</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B50" s="2">
-        <v>1750</v>
+        <v>32</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="B51" s="2">
-        <v>1769</v>
+        <v>172</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B52" s="2">
-        <v>1773</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B53" s="2">
-        <v>1795</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B54" s="2">
-        <v>1796</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B55" s="2">
-        <v>1822</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B56" s="2">
-        <v>69</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B57" s="2">
-        <v>22</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B58" s="2">
-        <v>155</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B59" s="2">
-        <v>171</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B60" s="2">
-        <v>201</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B61" s="2">
-        <v>270</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>